<commit_message>
great update, all problem fixed
</commit_message>
<xml_diff>
--- a/气象/冷站PK每日记录.xlsx
+++ b/气象/冷站PK每日记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5962FE11-ABAF-436B-9060-AA12F2D2D502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1E8D1A-826A-4D40-B555-67E5CD38CCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{ECFF787E-807D-4BE3-A541-0E06AE4591BB}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="301">
   <si>
     <t>地点</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1814,10 +1814,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>陶松臣格勒</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2746,6 +2742,9 @@
     <xf numFmtId="0" fontId="52" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2794,42 +2793,11 @@
     <xf numFmtId="0" fontId="41" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4361EE"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <b/>
@@ -2871,39 +2839,6 @@
         <i val="0"/>
         <color rgb="FF4361EE"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3232,7 +3167,7 @@
   <dimension ref="A1:BH48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3301,12 +3236,8 @@
       <c r="F2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="4">
-        <v>-32.299999999999997</v>
-      </c>
-      <c r="H2" s="4">
-        <v>-18.3</v>
-      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
       <c r="I2" s="6" t="s">
         <v>114</v>
       </c>
@@ -3324,145 +3255,145 @@
       </c>
       <c r="N2" cm="1">
         <f t="array" ref="N2:BH2">TRANSPOSE(G2:G48)</f>
-        <v>-32.299999999999997</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>-21.9</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>-33.799999999999997</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>-31.5</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>-31</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>-23.1</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>-21.2</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>-23.2</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>-25.1</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>-32.200000000000003</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>-32</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>-36.799999999999997</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>-29.2</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>-17.5</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>-22</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>-22.7</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>-28</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>-26.8</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>-26.5</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>-29.9</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>-35.299999999999997</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>-30.7</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>-15.5</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>-30.1</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>-28.2</v>
+        <v>0</v>
       </c>
       <c r="AN2">
-        <v>-19.2</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>-10.5</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>-5.2</v>
+        <v>0</v>
       </c>
       <c r="AQ2">
-        <v>-21</v>
+        <v>0</v>
       </c>
       <c r="AR2">
-        <v>-3.4</v>
+        <v>0</v>
       </c>
       <c r="AS2">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="AT2">
-        <v>-8.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="AU2">
-        <v>-6.7</v>
+        <v>0</v>
       </c>
       <c r="AV2">
-        <v>-4.5</v>
+        <v>0</v>
       </c>
       <c r="AW2">
-        <v>-5.8</v>
+        <v>0</v>
       </c>
       <c r="AX2">
-        <v>-7.8</v>
+        <v>0</v>
       </c>
       <c r="AY2">
-        <v>-16.3</v>
+        <v>0</v>
       </c>
       <c r="AZ2">
-        <v>-26.2</v>
+        <v>0</v>
       </c>
       <c r="BA2">
-        <v>-14.2</v>
+        <v>0</v>
       </c>
       <c r="BB2">
-        <v>-10.199999999999999</v>
+        <v>0</v>
       </c>
       <c r="BC2">
-        <v>-10.3</v>
+        <v>0</v>
       </c>
       <c r="BD2">
-        <v>-8.8000000000000007</v>
+        <v>0</v>
       </c>
       <c r="BE2">
-        <v>-10.5</v>
+        <v>0</v>
       </c>
       <c r="BF2">
-        <v>-13.2</v>
+        <v>0</v>
       </c>
       <c r="BG2">
-        <v>-22.5</v>
+        <v>0</v>
       </c>
       <c r="BH2">
-        <v>-27.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.4">
@@ -3482,12 +3413,8 @@
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4">
-        <v>-21.9</v>
-      </c>
-      <c r="H3" s="4">
-        <v>-4.0999999999999996</v>
-      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
       <c r="I3" s="6" t="s">
         <v>38</v>
       </c>
@@ -3505,145 +3432,145 @@
       </c>
       <c r="N3" cm="1">
         <f t="array" ref="N3:BH3">TRANSPOSE(H2:H48)</f>
-        <v>-18.3</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>-4.0999999999999996</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>-14.8</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>-11.6</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>-15.8</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>-11.7</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>-5.7</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>-1.9</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>-4.8</v>
-      </c>
-      <c r="W3" t="str">
-        <v>无</v>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>-10.4</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>-8.9</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>-11.5</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>-8.5</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <v>-7.4</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>-11.1</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>-15.3</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>-12.2</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>-10.6</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <v>-17.399999999999999</v>
+        <v>0</v>
       </c>
       <c r="AK3">
-        <v>-1.3</v>
+        <v>0</v>
       </c>
       <c r="AL3">
-        <v>-4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="AN3">
-        <v>-7.8</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>-1.6</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="AQ3">
-        <v>-9.6</v>
+        <v>0</v>
       </c>
       <c r="AR3">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="AS3">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="AT3">
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="AU3">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="AV3">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="AW3">
-        <v>5.3</v>
+        <v>0</v>
       </c>
       <c r="AX3">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="AY3">
-        <v>-6.1</v>
+        <v>0</v>
       </c>
       <c r="AZ3">
-        <v>-7.1</v>
+        <v>0</v>
       </c>
       <c r="BA3">
-        <v>-4.8</v>
+        <v>0</v>
       </c>
       <c r="BB3">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="BC3">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="BD3">
-        <v>-1.6</v>
+        <v>0</v>
       </c>
       <c r="BE3">
-        <v>-3.3</v>
+        <v>0</v>
       </c>
       <c r="BF3">
-        <v>-4.8</v>
+        <v>0</v>
       </c>
       <c r="BG3">
-        <v>-2.6</v>
+        <v>0</v>
       </c>
       <c r="BH3">
-        <v>-9.3000000000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.4">
@@ -3663,12 +3590,8 @@
       <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="4">
-        <v>-33.799999999999997</v>
-      </c>
-      <c r="H4" s="4">
-        <v>-14.8</v>
-      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="6" t="s">
         <v>117</v>
       </c>
@@ -3699,12 +3622,8 @@
       <c r="F5" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G5" s="4">
-        <v>-31.5</v>
-      </c>
-      <c r="H5" s="4">
-        <v>-11.6</v>
-      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
       <c r="I5" s="6" t="s">
         <v>40</v>
       </c>
@@ -3744,12 +3663,8 @@
       <c r="F6" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="G6" s="4">
-        <v>-31</v>
-      </c>
-      <c r="H6" s="4">
-        <v>-15.8</v>
-      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
       <c r="I6" s="6" t="s">
         <v>115</v>
       </c>
@@ -3789,12 +3704,8 @@
       <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="4">
-        <v>-24</v>
-      </c>
-      <c r="H7" s="4">
-        <v>-11.7</v>
-      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7" s="6" t="s">
         <v>113</v>
       </c>
@@ -3834,12 +3745,8 @@
       <c r="F8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="4">
-        <v>-23.1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>-5.7</v>
-      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="6" t="s">
         <v>120</v>
       </c>
@@ -3877,12 +3784,8 @@
       <c r="F9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="4">
-        <v>-21.2</v>
-      </c>
-      <c r="H9" s="4">
-        <v>-1.9</v>
-      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
       <c r="I9" s="6" t="s">
         <v>119</v>
       </c>
@@ -3911,12 +3814,8 @@
       <c r="F10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="4">
-        <v>-23.2</v>
-      </c>
-      <c r="H10" s="4">
-        <v>-4.8</v>
-      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
       <c r="I10" s="6" t="s">
         <v>100</v>
       </c>
@@ -3945,12 +3844,8 @@
       <c r="F11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="4">
-        <v>-25.1</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>286</v>
-      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
       <c r="I11" s="6" t="s">
         <v>54</v>
       </c>
@@ -3979,12 +3874,8 @@
       <c r="F12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="4">
-        <v>-32.200000000000003</v>
-      </c>
-      <c r="H12" s="4">
-        <v>-10.4</v>
-      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="6" t="s">
         <v>28</v>
       </c>
@@ -4013,12 +3904,8 @@
       <c r="F13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="4">
-        <v>-32</v>
-      </c>
-      <c r="H13" s="4">
-        <v>-8.9</v>
-      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
       <c r="I13" s="6" t="s">
         <v>28</v>
       </c>
@@ -4047,12 +3934,8 @@
       <c r="F14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="4">
-        <v>-36.799999999999997</v>
-      </c>
-      <c r="H14" s="4">
-        <v>-11.5</v>
-      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
       <c r="I14" s="6" t="s">
         <v>28</v>
       </c>
@@ -4081,12 +3964,8 @@
       <c r="F15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="G15" s="4">
-        <v>-29.2</v>
-      </c>
-      <c r="H15" s="4">
-        <v>-8.5</v>
-      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
       <c r="I15" s="6" t="s">
         <v>32</v>
       </c>
@@ -4115,12 +3994,8 @@
       <c r="F16" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="4">
-        <v>-17.5</v>
-      </c>
-      <c r="H16" s="4">
-        <v>-1</v>
-      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
       <c r="I16" s="6" t="s">
         <v>96</v>
       </c>
@@ -4149,12 +4024,8 @@
       <c r="F17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="4">
-        <v>-22</v>
-      </c>
-      <c r="H17" s="4">
-        <v>-7.4</v>
-      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
       <c r="I17" s="6" t="s">
         <v>161</v>
       </c>
@@ -4183,12 +4054,8 @@
       <c r="F18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="4">
-        <v>-22.7</v>
-      </c>
-      <c r="H18" s="4">
-        <v>-11.1</v>
-      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18" s="6" t="s">
         <v>22</v>
       </c>
@@ -4217,12 +4084,8 @@
       <c r="F19" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="4">
-        <v>-28</v>
-      </c>
-      <c r="H19" s="4">
-        <v>-15.3</v>
-      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
       <c r="I19" s="6" t="s">
         <v>114</v>
       </c>
@@ -4251,12 +4114,8 @@
       <c r="F20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="13">
-        <v>-26.8</v>
-      </c>
-      <c r="H20" s="13">
-        <v>-12.2</v>
-      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="6" t="s">
         <v>113</v>
       </c>
@@ -4285,12 +4144,8 @@
       <c r="F21" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="13">
-        <v>-26.5</v>
-      </c>
-      <c r="H21" s="13">
-        <v>-15</v>
-      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="6" t="s">
         <v>115</v>
       </c>
@@ -4319,12 +4174,8 @@
       <c r="F22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="13">
-        <v>-29.9</v>
-      </c>
-      <c r="H22" s="13">
-        <v>-10.6</v>
-      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="6" t="s">
         <v>40</v>
       </c>
@@ -4355,12 +4206,8 @@
       <c r="F23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="13">
-        <v>-35.299999999999997</v>
-      </c>
-      <c r="H23" s="13">
-        <v>-6</v>
-      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="6" t="s">
         <v>36</v>
       </c>
@@ -4391,12 +4238,8 @@
       <c r="F24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="13">
-        <v>-30.7</v>
-      </c>
-      <c r="H24" s="13">
-        <v>-17.399999999999999</v>
-      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="6" t="s">
         <v>118</v>
       </c>
@@ -4425,12 +4268,8 @@
       <c r="F25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="4">
-        <v>-15.5</v>
-      </c>
-      <c r="H25" s="4">
-        <v>-1.3</v>
-      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
       <c r="I25" s="6" t="s">
         <v>38</v>
       </c>
@@ -4461,12 +4300,8 @@
       <c r="F26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="4">
-        <v>-30.1</v>
-      </c>
-      <c r="H26" s="4">
-        <v>-4.4000000000000004</v>
-      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
       <c r="I26" s="6" t="s">
         <v>2</v>
       </c>
@@ -4495,12 +4330,8 @@
       <c r="F27" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G27" s="4">
-        <v>-28.2</v>
-      </c>
-      <c r="H27" s="4">
-        <v>-4</v>
-      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
       <c r="I27" s="6" t="s">
         <v>2</v>
       </c>
@@ -4529,12 +4360,8 @@
       <c r="F28" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="4">
-        <v>-19.2</v>
-      </c>
-      <c r="H28" s="4">
-        <v>-7.8</v>
-      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="I28" s="6" t="s">
         <v>75</v>
       </c>
@@ -4565,12 +4392,8 @@
       <c r="F29" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G29" s="4">
-        <v>-10.5</v>
-      </c>
-      <c r="H29" s="4">
-        <v>-1.6</v>
-      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
       <c r="I29" s="6" t="s">
         <v>22</v>
       </c>
@@ -4599,12 +4422,8 @@
       <c r="F30" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="4">
-        <v>-5.2</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1.3</v>
-      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
       <c r="I30" s="6" t="s">
         <v>21</v>
       </c>
@@ -4635,12 +4454,8 @@
       <c r="F31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="4">
-        <v>-21</v>
-      </c>
-      <c r="H31" s="4">
-        <v>-9.6</v>
-      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
       <c r="I31" s="6" t="s">
         <v>21</v>
       </c>
@@ -4669,12 +4484,8 @@
       <c r="F32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="4">
-        <v>-3.4</v>
-      </c>
-      <c r="H32" s="4">
-        <v>3.4</v>
-      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
       <c r="I32" s="6"/>
       <c r="J32" s="13" t="s">
         <v>129</v>
@@ -4701,12 +4512,8 @@
       <c r="F33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="4">
-        <v>-12</v>
-      </c>
-      <c r="H33" s="4">
-        <v>2.2000000000000002</v>
-      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
       <c r="I33" s="6"/>
       <c r="J33" s="14" t="s">
         <v>131</v>
@@ -4735,12 +4542,8 @@
       <c r="F34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G34" s="4">
-        <v>-8.1999999999999993</v>
-      </c>
-      <c r="H34" s="4">
-        <v>-0.8</v>
-      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
       <c r="I34" s="6"/>
       <c r="J34" s="14" t="s">
         <v>131</v>
@@ -4769,12 +4572,8 @@
       <c r="F35" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="4">
-        <v>-6.7</v>
-      </c>
-      <c r="H35" s="4">
-        <v>1.9</v>
-      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
       <c r="I35" s="6" t="s">
         <v>47</v>
       </c>
@@ -4805,12 +4604,8 @@
       <c r="F36" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="4">
-        <v>-4.5</v>
-      </c>
-      <c r="H36" s="4">
-        <v>2.6</v>
-      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
       <c r="I36" s="6" t="s">
         <v>45</v>
       </c>
@@ -4841,12 +4636,8 @@
       <c r="F37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G37" s="4">
-        <v>-5.8</v>
-      </c>
-      <c r="H37" s="4">
-        <v>5.3</v>
-      </c>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
       <c r="I37" s="6"/>
       <c r="J37" s="14" t="s">
         <v>130</v>
@@ -4875,12 +4666,8 @@
       <c r="F38" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G38" s="4">
-        <v>-7.8</v>
-      </c>
-      <c r="H38" s="4">
-        <v>2.8</v>
-      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
       <c r="I38" s="6"/>
       <c r="J38" s="14" t="s">
         <v>130</v>
@@ -4909,12 +4696,8 @@
       <c r="F39" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="4">
-        <v>-16.3</v>
-      </c>
-      <c r="H39" s="4">
-        <v>-6.1</v>
-      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
       <c r="I39" s="6" t="s">
         <v>43</v>
       </c>
@@ -4943,12 +4726,8 @@
       <c r="F40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G40" s="4">
-        <v>-26.2</v>
-      </c>
-      <c r="H40" s="4">
-        <v>-7.1</v>
-      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
       <c r="I40" s="6" t="s">
         <v>2</v>
       </c>
@@ -4977,12 +4756,8 @@
       <c r="F41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G41" s="4">
-        <v>-14.2</v>
-      </c>
-      <c r="H41" s="4">
-        <v>-4.8</v>
-      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
       <c r="I41" s="6" t="s">
         <v>2</v>
       </c>
@@ -5011,12 +4786,8 @@
       <c r="F42" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="4">
-        <v>-10.199999999999999</v>
-      </c>
-      <c r="H42" s="4">
-        <v>1.5</v>
-      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
       <c r="I42" s="6" t="s">
         <v>65</v>
       </c>
@@ -5045,12 +4816,8 @@
       <c r="F43" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="4">
-        <v>-10.3</v>
-      </c>
-      <c r="H43" s="4">
-        <v>2.5</v>
-      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
       <c r="I43" s="6" t="s">
         <v>65</v>
       </c>
@@ -5079,12 +4846,8 @@
       <c r="F44" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G44" s="4">
-        <v>-8.8000000000000007</v>
-      </c>
-      <c r="H44" s="4">
-        <v>-1.6</v>
-      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
       <c r="I44" s="6" t="s">
         <v>22</v>
       </c>
@@ -5113,12 +4876,8 @@
       <c r="F45" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="4">
-        <v>-10.5</v>
-      </c>
-      <c r="H45" s="4">
-        <v>-3.3</v>
-      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
       <c r="I45" s="6" t="s">
         <v>21</v>
       </c>
@@ -5147,12 +4906,8 @@
       <c r="F46" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G46" s="4">
-        <v>-13.2</v>
-      </c>
-      <c r="H46" s="4">
-        <v>-4.8</v>
-      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
       <c r="I46" s="6" t="s">
         <v>21</v>
       </c>
@@ -5183,12 +4938,8 @@
       <c r="F47" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G47" s="4">
-        <v>-22.5</v>
-      </c>
-      <c r="H47" s="4">
-        <v>-2.6</v>
-      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
       <c r="I47" s="6" t="s">
         <v>2</v>
       </c>
@@ -5217,12 +4968,8 @@
       <c r="F48" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G48" s="4">
-        <v>-27.4</v>
-      </c>
-      <c r="H48" s="4">
-        <v>-9.3000000000000007</v>
-      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
       <c r="I48" s="6" t="s">
         <v>2</v>
       </c>
@@ -5265,34 +5012,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="61" t="s">
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="62" t="s">
         <v>246</v>
       </c>
-      <c r="F1" s="64">
-        <v>45721</v>
-      </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="62" t="s">
+      <c r="F1" s="65">
+        <v>45725</v>
+      </c>
+      <c r="G1" s="66"/>
+      <c r="H1" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="63"/>
+      <c r="I1" s="64"/>
     </row>
     <row r="2" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="60" t="s">
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="61" t="s">
         <v>250</v>
       </c>
-      <c r="I2" s="60"/>
+      <c r="I2" s="61"/>
       <c r="K2" s="21" t="s">
         <v>176</v>
       </c>
@@ -5304,7 +5051,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="59"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="51" t="s">
         <v>90</v>
       </c>
@@ -5340,7 +5087,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="53">
         <v>1</v>
       </c>
@@ -5356,12 +5103,8 @@
       <c r="F4" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="36">
-        <v>-32.299999999999997</v>
-      </c>
-      <c r="H4" s="56">
-        <v>-18.3</v>
-      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="34" t="s">
         <v>174</v>
       </c>
@@ -5376,7 +5119,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="59"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="53">
         <v>2</v>
       </c>
@@ -5390,43 +5133,37 @@
       <c r="F5" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="36">
-        <v>-21.9</v>
-      </c>
-      <c r="H5" s="36">
-        <v>-4.0999999999999996</v>
-      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
       <c r="I5" s="34" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="59"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="53">
         <v>3</v>
       </c>
       <c r="C6" s="52">
         <v>3</v>
       </c>
-      <c r="D6" s="52"/>
+      <c r="D6" s="52">
+        <v>0</v>
+      </c>
       <c r="E6" s="32" t="s">
         <v>215</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="36">
-        <v>-33.799999999999997</v>
-      </c>
-      <c r="H6" s="36">
-        <v>-14.8</v>
-      </c>
+      <c r="G6" s="57"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="34" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="59"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="53">
         <v>4</v>
       </c>
@@ -5440,18 +5177,14 @@
       <c r="F7" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="G7" s="36">
-        <v>-31.5</v>
-      </c>
-      <c r="H7" s="36">
-        <v>-11.6</v>
-      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="34" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="59"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="53">
         <v>5</v>
       </c>
@@ -5465,18 +5198,14 @@
       <c r="F8" s="45" t="s">
         <v>183</v>
       </c>
-      <c r="G8" s="36">
-        <v>-31</v>
-      </c>
-      <c r="H8" s="36">
-        <v>-15.8</v>
-      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="34" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="59"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="53">
         <v>6</v>
       </c>
@@ -5490,18 +5219,14 @@
       <c r="F9" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="36">
-        <v>-24</v>
-      </c>
-      <c r="H9" s="36">
-        <v>-11.7</v>
-      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="34" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="59"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="53">
         <v>7</v>
       </c>
@@ -5515,18 +5240,14 @@
       <c r="F10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="36">
-        <v>-23.1</v>
-      </c>
-      <c r="H10" s="36">
-        <v>-5.7</v>
-      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="34" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="59"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="53">
         <v>8</v>
       </c>
@@ -5540,18 +5261,14 @@
       <c r="F11" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="36">
-        <v>-21.2</v>
-      </c>
-      <c r="H11" s="36">
-        <v>-1.9</v>
-      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="34" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="59"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="53">
         <v>9</v>
       </c>
@@ -5565,18 +5282,14 @@
       <c r="F12" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="G12" s="36">
-        <v>-23.2</v>
-      </c>
-      <c r="H12" s="36">
-        <v>-4.8</v>
-      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="34" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="59"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="53">
         <v>10</v>
       </c>
@@ -5590,18 +5303,14 @@
       <c r="F13" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="G13" s="57">
-        <v>-25.1</v>
-      </c>
-      <c r="H13" s="36" t="s">
-        <v>245</v>
-      </c>
+      <c r="G13" s="57"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="34" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="59"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="53">
         <v>11</v>
       </c>
@@ -5615,18 +5324,14 @@
       <c r="F14" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="36">
-        <v>-32.200000000000003</v>
-      </c>
-      <c r="H14" s="36">
-        <v>-10.4</v>
-      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="34" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="59"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="53">
         <v>12</v>
       </c>
@@ -5640,18 +5345,14 @@
       <c r="F15" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="36">
-        <v>-32</v>
-      </c>
-      <c r="H15" s="36">
-        <v>-8.9</v>
-      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="34" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="59"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="53">
         <v>13</v>
       </c>
@@ -5667,18 +5368,14 @@
       <c r="F16" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G16" s="56">
-        <v>-36.799999999999997</v>
-      </c>
-      <c r="H16" s="36">
-        <v>-11.5</v>
-      </c>
+      <c r="G16" s="56"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="34" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="59"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="53">
         <v>14</v>
       </c>
@@ -5692,18 +5389,14 @@
       <c r="F17" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="G17" s="36">
-        <v>-29.2</v>
-      </c>
-      <c r="H17" s="36">
-        <v>-8.5</v>
-      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="34" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="59"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="53">
         <v>15</v>
       </c>
@@ -5717,18 +5410,14 @@
       <c r="F18" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="36">
-        <v>-17.5</v>
-      </c>
-      <c r="H18" s="36">
-        <v>-1</v>
-      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="59"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="53">
         <v>16</v>
       </c>
@@ -5742,18 +5431,14 @@
       <c r="F19" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="36">
-        <v>-22</v>
-      </c>
-      <c r="H19" s="36">
-        <v>-7.4</v>
-      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
       <c r="I19" s="34" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="59"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="53">
         <v>17</v>
       </c>
@@ -5767,18 +5452,14 @@
       <c r="F20" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="36">
-        <v>-22.7</v>
-      </c>
-      <c r="H20" s="36">
-        <v>-11.1</v>
-      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
       <c r="I20" s="34" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="59"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="53">
         <v>18</v>
       </c>
@@ -5792,18 +5473,14 @@
       <c r="F21" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="36">
-        <v>-28</v>
-      </c>
-      <c r="H21" s="36">
-        <v>-15.3</v>
-      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
       <c r="I21" s="34" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="59"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="53">
         <v>19</v>
       </c>
@@ -5817,18 +5494,14 @@
       <c r="F22" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="36">
-        <v>-26.8</v>
-      </c>
-      <c r="H22" s="36">
-        <v>-12.2</v>
-      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="34" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="59"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="53">
         <v>20</v>
       </c>
@@ -5842,18 +5515,14 @@
       <c r="F23" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="36">
-        <v>-26.5</v>
-      </c>
-      <c r="H23" s="36">
-        <v>-15</v>
-      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
       <c r="I23" s="34" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="59"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="53">
         <v>21</v>
       </c>
@@ -5867,45 +5536,35 @@
       <c r="F24" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="36">
-        <v>-29.9</v>
-      </c>
-      <c r="H24" s="36">
-        <v>-10.6</v>
-      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="34" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="59"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="53">
         <v>22</v>
       </c>
       <c r="C25" s="52">
         <v>3</v>
       </c>
-      <c r="D25" s="52">
-        <v>0</v>
-      </c>
+      <c r="D25" s="52"/>
       <c r="E25" s="32" t="s">
         <v>215</v>
       </c>
       <c r="F25" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="36">
-        <v>-35.299999999999997</v>
-      </c>
-      <c r="H25" s="36">
-        <v>-6</v>
-      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
       <c r="I25" s="34" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="59"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="53">
         <v>23</v>
       </c>
@@ -5919,18 +5578,14 @@
       <c r="F26" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="36">
-        <v>-30.7</v>
-      </c>
-      <c r="H26" s="36">
-        <v>-17.399999999999999</v>
-      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
       <c r="I26" s="34" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="59"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="53">
         <v>24</v>
       </c>
@@ -5944,45 +5599,35 @@
       <c r="F27" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="36">
-        <v>-15.5</v>
-      </c>
-      <c r="H27" s="36">
-        <v>-1.3</v>
-      </c>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
       <c r="I27" s="34" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="59"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="53">
         <v>25</v>
       </c>
       <c r="C28" s="52">
         <v>1</v>
       </c>
-      <c r="D28" s="52">
-        <v>0</v>
-      </c>
+      <c r="D28" s="52"/>
       <c r="E28" s="30" t="s">
         <v>212</v>
       </c>
       <c r="F28" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="G28" s="36">
-        <v>-30.1</v>
-      </c>
-      <c r="H28" s="36">
-        <v>-4.4000000000000004</v>
-      </c>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
       <c r="I28" s="34" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="59"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="53">
         <v>26</v>
       </c>
@@ -5998,18 +5643,14 @@
       <c r="F29" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G29" s="36">
-        <v>-28.2</v>
-      </c>
-      <c r="H29" s="36">
-        <v>-4</v>
-      </c>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
       <c r="I29" s="34" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="59"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="53">
         <v>27</v>
       </c>
@@ -6023,18 +5664,14 @@
       <c r="F30" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="36">
-        <v>-19.2</v>
-      </c>
-      <c r="H30" s="36">
-        <v>-7.8</v>
-      </c>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
       <c r="I30" s="34" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="59"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="53">
         <v>28</v>
       </c>
@@ -6050,18 +5687,14 @@
       <c r="F31" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="G31" s="36">
-        <v>-10.5</v>
-      </c>
-      <c r="H31" s="36">
-        <v>-1.6</v>
-      </c>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
       <c r="I31" s="34" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="59"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="53">
         <v>29</v>
       </c>
@@ -6075,18 +5708,14 @@
       <c r="F32" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="36">
-        <v>-5.2</v>
-      </c>
-      <c r="H32" s="36">
-        <v>1.3</v>
-      </c>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
       <c r="I32" s="34" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="59"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="53">
         <v>30</v>
       </c>
@@ -6102,18 +5731,14 @@
       <c r="F33" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="36">
-        <v>-21</v>
-      </c>
-      <c r="H33" s="36">
-        <v>-9.6</v>
-      </c>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
       <c r="I33" s="34" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="59"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="53">
         <v>31</v>
       </c>
@@ -6127,18 +5752,14 @@
       <c r="F34" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="G34" s="36">
-        <v>-3.4</v>
-      </c>
-      <c r="H34" s="36">
-        <v>3.4</v>
-      </c>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
       <c r="I34" s="34" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="59"/>
+      <c r="A35" s="60"/>
       <c r="B35" s="53">
         <v>32</v>
       </c>
@@ -6152,16 +5773,12 @@
       <c r="F35" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="G35" s="36">
-        <v>-12</v>
-      </c>
-      <c r="H35" s="36">
-        <v>2.2000000000000002</v>
-      </c>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
       <c r="I35" s="34"/>
     </row>
     <row r="36" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="59"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="53">
         <v>33</v>
       </c>
@@ -6177,16 +5794,12 @@
       <c r="F36" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="G36" s="36">
-        <v>-8.1999999999999993</v>
-      </c>
-      <c r="H36" s="36">
-        <v>-0.8</v>
-      </c>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
       <c r="I36" s="34"/>
     </row>
     <row r="37" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="59"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="53">
         <v>34</v>
       </c>
@@ -6202,18 +5815,14 @@
       <c r="F37" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="G37" s="36">
-        <v>-6.7</v>
-      </c>
-      <c r="H37" s="36">
-        <v>1.9</v>
-      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
       <c r="I37" s="34" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="59"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="53">
         <v>35</v>
       </c>
@@ -6229,18 +5838,14 @@
       <c r="F38" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="G38" s="36">
-        <v>-4.5</v>
-      </c>
-      <c r="H38" s="36">
-        <v>2.6</v>
-      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
       <c r="I38" s="34" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="59"/>
+      <c r="A39" s="60"/>
       <c r="B39" s="53">
         <v>36</v>
       </c>
@@ -6256,16 +5861,12 @@
       <c r="F39" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="G39" s="36">
-        <v>-5.8</v>
-      </c>
-      <c r="H39" s="36">
-        <v>5.3</v>
-      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
       <c r="I39" s="34"/>
     </row>
     <row r="40" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="59"/>
+      <c r="A40" s="60"/>
       <c r="B40" s="53">
         <v>37</v>
       </c>
@@ -6281,41 +5882,35 @@
       <c r="F40" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="G40" s="36">
-        <v>-7.8</v>
-      </c>
-      <c r="H40" s="36">
-        <v>2.8</v>
-      </c>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
       <c r="I40" s="34"/>
     </row>
     <row r="41" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="59"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="53">
         <v>38</v>
       </c>
       <c r="C41" s="52">
         <v>1</v>
       </c>
-      <c r="D41" s="52"/>
+      <c r="D41" s="52">
+        <v>0</v>
+      </c>
       <c r="E41" s="30" t="s">
         <v>208</v>
       </c>
       <c r="F41" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="G41" s="36">
-        <v>-16.3</v>
-      </c>
-      <c r="H41" s="36">
-        <v>-6.1</v>
-      </c>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
       <c r="I41" s="34" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="59"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="53">
         <v>39</v>
       </c>
@@ -6329,18 +5924,14 @@
       <c r="F42" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="G42" s="36">
-        <v>-26.2</v>
-      </c>
-      <c r="H42" s="36">
-        <v>-7.1</v>
-      </c>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
       <c r="I42" s="34" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="59"/>
+      <c r="A43" s="60"/>
       <c r="B43" s="53">
         <v>40</v>
       </c>
@@ -6354,18 +5945,14 @@
       <c r="F43" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="G43" s="36">
-        <v>-14.2</v>
-      </c>
-      <c r="H43" s="36">
-        <v>-4.8</v>
-      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
       <c r="I43" s="34" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="59"/>
+      <c r="A44" s="60"/>
       <c r="B44" s="53">
         <v>41</v>
       </c>
@@ -6379,18 +5966,14 @@
       <c r="F44" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="G44" s="36">
-        <v>-10.199999999999999</v>
-      </c>
-      <c r="H44" s="36">
-        <v>1.5</v>
-      </c>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="34" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="59"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="53">
         <v>42</v>
       </c>
@@ -6404,18 +5987,14 @@
       <c r="F45" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="G45" s="36">
-        <v>-10.3</v>
-      </c>
-      <c r="H45" s="36">
-        <v>2.5</v>
-      </c>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
       <c r="I45" s="34" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="59"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="53">
         <v>43</v>
       </c>
@@ -6429,18 +6008,14 @@
       <c r="F46" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="36">
-        <v>-8.8000000000000007</v>
-      </c>
-      <c r="H46" s="36">
-        <v>-1.6</v>
-      </c>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
       <c r="I46" s="34" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="59"/>
+      <c r="A47" s="60"/>
       <c r="B47" s="53">
         <v>44</v>
       </c>
@@ -6454,18 +6029,14 @@
       <c r="F47" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="G47" s="36">
-        <v>-10.5</v>
-      </c>
-      <c r="H47" s="36">
-        <v>-3.3</v>
-      </c>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
       <c r="I47" s="34" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="59"/>
+      <c r="A48" s="60"/>
       <c r="B48" s="53">
         <v>45</v>
       </c>
@@ -6479,18 +6050,14 @@
       <c r="F48" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="G48" s="36">
-        <v>-13.2</v>
-      </c>
-      <c r="H48" s="36">
-        <v>-4.8</v>
-      </c>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
       <c r="I48" s="34" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="59"/>
+      <c r="A49" s="60"/>
       <c r="B49" s="53">
         <v>46</v>
       </c>
@@ -6504,18 +6071,14 @@
       <c r="F49" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="36">
-        <v>-22.5</v>
-      </c>
-      <c r="H49" s="36">
-        <v>-2.6</v>
-      </c>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
       <c r="I49" s="34" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="59"/>
+      <c r="A50" s="60"/>
       <c r="B50" s="53">
         <v>47</v>
       </c>
@@ -6529,21 +6092,17 @@
       <c r="F50" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="G50" s="36">
-        <v>-27.4</v>
-      </c>
-      <c r="H50" s="36">
-        <v>-9.3000000000000007</v>
-      </c>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
       <c r="I50" s="34" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="59"/>
+      <c r="A51" s="60"/>
     </row>
     <row r="52" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="59"/>
+      <c r="A52" s="60"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I50">
@@ -6592,8 +6151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6452CB3-0983-4391-8A7D-2C5221219E76}">
   <dimension ref="A1:AV344"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -17409,15 +16968,438 @@
       <c r="A75" s="16">
         <v>45722</v>
       </c>
+      <c r="B75">
+        <v>-31.7</v>
+      </c>
+      <c r="C75">
+        <v>-17.5</v>
+      </c>
+      <c r="D75">
+        <v>-30.4</v>
+      </c>
+      <c r="E75">
+        <v>-31.9</v>
+      </c>
+      <c r="F75">
+        <v>-25.4</v>
+      </c>
+      <c r="G75">
+        <v>-24.4</v>
+      </c>
+      <c r="H75">
+        <v>-17.3</v>
+      </c>
+      <c r="I75">
+        <v>-18.3</v>
+      </c>
+      <c r="J75">
+        <v>-23.2</v>
+      </c>
+      <c r="K75">
+        <v>-22.4</v>
+      </c>
+      <c r="L75">
+        <v>-33.4</v>
+      </c>
+      <c r="M75">
+        <v>-33.5</v>
+      </c>
+      <c r="N75">
+        <v>-36.4</v>
+      </c>
+      <c r="O75">
+        <v>-27.6</v>
+      </c>
+      <c r="P75">
+        <v>-26.1</v>
+      </c>
+      <c r="Q75">
+        <v>-22.6</v>
+      </c>
+      <c r="R75">
+        <v>-23.4</v>
+      </c>
+      <c r="S75">
+        <v>-27.5</v>
+      </c>
+      <c r="T75">
+        <v>-26.3</v>
+      </c>
+      <c r="U75">
+        <v>-27.7</v>
+      </c>
+      <c r="V75">
+        <v>-29.4</v>
+      </c>
+      <c r="W75">
+        <v>-32</v>
+      </c>
+      <c r="X75">
+        <v>-30.3</v>
+      </c>
+      <c r="Y75">
+        <v>-11.6</v>
+      </c>
+      <c r="Z75">
+        <v>-29.1</v>
+      </c>
+      <c r="AA75">
+        <v>-31.1</v>
+      </c>
+      <c r="AB75">
+        <v>-22.6</v>
+      </c>
+      <c r="AC75">
+        <v>-8.6</v>
+      </c>
+      <c r="AD75">
+        <v>-5.9</v>
+      </c>
+      <c r="AE75">
+        <v>-29.1</v>
+      </c>
+      <c r="AF75">
+        <v>-7.8</v>
+      </c>
+      <c r="AG75">
+        <v>-7</v>
+      </c>
+      <c r="AH75">
+        <v>-15.2</v>
+      </c>
+      <c r="AI75">
+        <v>-11.2</v>
+      </c>
+      <c r="AJ75">
+        <v>-8.6</v>
+      </c>
+      <c r="AK75">
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="AL75">
+        <v>-14.5</v>
+      </c>
+      <c r="AM75">
+        <v>-26.2</v>
+      </c>
+      <c r="AN75">
+        <v>-30</v>
+      </c>
+      <c r="AO75">
+        <v>-22.8</v>
+      </c>
+      <c r="AP75">
+        <v>-16.8</v>
+      </c>
+      <c r="AQ75">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="AR75">
+        <v>-17</v>
+      </c>
+      <c r="AS75">
+        <v>-12.5</v>
+      </c>
+      <c r="AT75">
+        <v>-12.9</v>
+      </c>
+      <c r="AU75">
+        <v>-27.3</v>
+      </c>
+      <c r="AV75">
+        <v>-28.2</v>
+      </c>
     </row>
     <row r="76" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A76" s="16">
         <v>45723</v>
       </c>
+      <c r="B76">
+        <v>-31.5</v>
+      </c>
+      <c r="C76">
+        <v>-20.2</v>
+      </c>
+      <c r="D76">
+        <v>-30.1</v>
+      </c>
+      <c r="E76">
+        <v>-33.200000000000003</v>
+      </c>
+      <c r="F76">
+        <v>-32.4</v>
+      </c>
+      <c r="G76">
+        <v>-25</v>
+      </c>
+      <c r="H76">
+        <v>-24.6</v>
+      </c>
+      <c r="I76">
+        <v>-17.5</v>
+      </c>
+      <c r="J76">
+        <v>-24.4</v>
+      </c>
+      <c r="K76">
+        <v>-25.7</v>
+      </c>
+      <c r="L76">
+        <v>-33.6</v>
+      </c>
+      <c r="M76">
+        <v>-35.9</v>
+      </c>
+      <c r="N76">
+        <v>-38.4</v>
+      </c>
+      <c r="O76">
+        <v>-30</v>
+      </c>
+      <c r="P76">
+        <v>-26.7</v>
+      </c>
+      <c r="Q76">
+        <v>-22.3</v>
+      </c>
+      <c r="R76">
+        <v>-24.7</v>
+      </c>
+      <c r="S76">
+        <v>-29.9</v>
+      </c>
+      <c r="T76">
+        <v>-26</v>
+      </c>
+      <c r="U76">
+        <v>-28.4</v>
+      </c>
+      <c r="V76">
+        <v>-30.8</v>
+      </c>
+      <c r="W76">
+        <v>-30.9</v>
+      </c>
+      <c r="X76">
+        <v>-29.8</v>
+      </c>
+      <c r="Y76">
+        <v>-13.7</v>
+      </c>
+      <c r="Z76">
+        <v>-32.799999999999997</v>
+      </c>
+      <c r="AA76">
+        <v>-29.7</v>
+      </c>
+      <c r="AB76">
+        <v>-19.2</v>
+      </c>
+      <c r="AC76">
+        <v>-7.4</v>
+      </c>
+      <c r="AD76">
+        <v>-7.8</v>
+      </c>
+      <c r="AE76">
+        <v>-29.9</v>
+      </c>
+      <c r="AF76">
+        <v>-5.5</v>
+      </c>
+      <c r="AG76">
+        <v>-9.1999999999999993</v>
+      </c>
+      <c r="AH76">
+        <v>-10.7</v>
+      </c>
+      <c r="AI76">
+        <v>-12.8</v>
+      </c>
+      <c r="AJ76">
+        <v>-10.7</v>
+      </c>
+      <c r="AK76">
+        <v>-10.3</v>
+      </c>
+      <c r="AL76">
+        <v>-6.1</v>
+      </c>
+      <c r="AM76">
+        <v>-29.7</v>
+      </c>
+      <c r="AN76">
+        <v>-32.700000000000003</v>
+      </c>
+      <c r="AO76">
+        <v>-16.2</v>
+      </c>
+      <c r="AP76">
+        <v>-24.3</v>
+      </c>
+      <c r="AQ76">
+        <v>-10.4</v>
+      </c>
+      <c r="AR76">
+        <v>-13.4</v>
+      </c>
+      <c r="AS76">
+        <v>-9.5</v>
+      </c>
+      <c r="AT76">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="AU76">
+        <v>-26.8</v>
+      </c>
+      <c r="AV76">
+        <v>-23.8</v>
+      </c>
     </row>
     <row r="77" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A77" s="16">
         <v>45724</v>
+      </c>
+      <c r="B77">
+        <v>-26.3</v>
+      </c>
+      <c r="C77">
+        <v>-19.3</v>
+      </c>
+      <c r="D77">
+        <v>-29.9</v>
+      </c>
+      <c r="E77">
+        <v>-20.5</v>
+      </c>
+      <c r="F77">
+        <v>-26.5</v>
+      </c>
+      <c r="G77">
+        <v>-19.7</v>
+      </c>
+      <c r="H77">
+        <v>-24.4</v>
+      </c>
+      <c r="I77">
+        <v>-19.899999999999999</v>
+      </c>
+      <c r="J77">
+        <v>-22.3</v>
+      </c>
+      <c r="K77">
+        <v>-21.6</v>
+      </c>
+      <c r="L77">
+        <v>-32.9</v>
+      </c>
+      <c r="M77">
+        <v>-36.1</v>
+      </c>
+      <c r="N77">
+        <v>-37.200000000000003</v>
+      </c>
+      <c r="O77">
+        <v>-31.5</v>
+      </c>
+      <c r="P77">
+        <v>-24.1</v>
+      </c>
+      <c r="Q77">
+        <v>-17.8</v>
+      </c>
+      <c r="R77">
+        <v>-14.7</v>
+      </c>
+      <c r="S77">
+        <v>-24</v>
+      </c>
+      <c r="T77">
+        <v>-21.2</v>
+      </c>
+      <c r="U77">
+        <v>-24.9</v>
+      </c>
+      <c r="V77">
+        <v>-17.8</v>
+      </c>
+      <c r="W77">
+        <v>-19.8</v>
+      </c>
+      <c r="X77">
+        <v>-23.6</v>
+      </c>
+      <c r="Y77">
+        <v>-10</v>
+      </c>
+      <c r="Z77">
+        <v>-26.6</v>
+      </c>
+      <c r="AA77">
+        <v>-28.3</v>
+      </c>
+      <c r="AB77">
+        <v>-23.1</v>
+      </c>
+      <c r="AC77">
+        <v>-2.9</v>
+      </c>
+      <c r="AD77">
+        <v>-6.4</v>
+      </c>
+      <c r="AE77">
+        <v>-19.8</v>
+      </c>
+      <c r="AF77">
+        <v>-7.1</v>
+      </c>
+      <c r="AG77">
+        <v>-9.3000000000000007</v>
+      </c>
+      <c r="AH77">
+        <v>-11.5</v>
+      </c>
+      <c r="AI77">
+        <v>-3.5</v>
+      </c>
+      <c r="AJ77">
+        <v>-3.1</v>
+      </c>
+      <c r="AK77">
+        <v>-1.2</v>
+      </c>
+      <c r="AL77">
+        <v>-11.4</v>
+      </c>
+      <c r="AM77">
+        <v>-29.8</v>
+      </c>
+      <c r="AN77">
+        <v>-26.8</v>
+      </c>
+      <c r="AO77">
+        <v>-20.399999999999999</v>
+      </c>
+      <c r="AP77">
+        <v>-25.2</v>
+      </c>
+      <c r="AQ77">
+        <v>-13.6</v>
+      </c>
+      <c r="AR77">
+        <v>-8.1</v>
+      </c>
+      <c r="AS77">
+        <v>-8.9</v>
+      </c>
+      <c r="AT77">
+        <v>-6.9</v>
+      </c>
+      <c r="AU77">
+        <v>-25.8</v>
+      </c>
+      <c r="AV77">
+        <v>-26.6</v>
       </c>
     </row>
     <row r="78" spans="1:48" x14ac:dyDescent="0.4">
@@ -18766,7 +18748,7 @@
   <dimension ref="A1:AV351"/>
   <sheetViews>
     <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -29582,15 +29564,438 @@
       <c r="A75" s="16">
         <v>45722</v>
       </c>
+      <c r="B75">
+        <v>-17.8</v>
+      </c>
+      <c r="C75">
+        <v>0.1</v>
+      </c>
+      <c r="D75">
+        <v>-11.4</v>
+      </c>
+      <c r="E75">
+        <v>-11.8</v>
+      </c>
+      <c r="F75">
+        <v>-13.8</v>
+      </c>
+      <c r="G75">
+        <v>-7.8</v>
+      </c>
+      <c r="H75">
+        <v>-1</v>
+      </c>
+      <c r="I75">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="J75">
+        <v>-6.3</v>
+      </c>
+      <c r="K75" t="s">
+        <v>245</v>
+      </c>
+      <c r="L75">
+        <v>-12.7</v>
+      </c>
+      <c r="M75">
+        <v>-10.1</v>
+      </c>
+      <c r="N75">
+        <v>-15.2</v>
+      </c>
+      <c r="O75">
+        <v>-7.1</v>
+      </c>
+      <c r="P75">
+        <v>-6.2</v>
+      </c>
+      <c r="Q75">
+        <v>-6.1</v>
+      </c>
+      <c r="R75">
+        <v>-10.4</v>
+      </c>
+      <c r="S75">
+        <v>-14.7</v>
+      </c>
+      <c r="T75">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="U75">
+        <v>-13.4</v>
+      </c>
+      <c r="V75">
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="W75">
+        <v>-6.5</v>
+      </c>
+      <c r="X75">
+        <v>-14.5</v>
+      </c>
+      <c r="Y75">
+        <v>1</v>
+      </c>
+      <c r="Z75">
+        <v>-7</v>
+      </c>
+      <c r="AA75">
+        <v>-4.2</v>
+      </c>
+      <c r="AB75">
+        <v>-7</v>
+      </c>
+      <c r="AC75">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AD75">
+        <v>-1.6</v>
+      </c>
+      <c r="AE75">
+        <v>-14.9</v>
+      </c>
+      <c r="AF75">
+        <v>4.7</v>
+      </c>
+      <c r="AG75">
+        <v>5.8</v>
+      </c>
+      <c r="AH75">
+        <v>2.1</v>
+      </c>
+      <c r="AI75">
+        <v>0.4</v>
+      </c>
+      <c r="AJ75">
+        <v>3.6</v>
+      </c>
+      <c r="AK75">
+        <v>4.3</v>
+      </c>
+      <c r="AL75">
+        <v>6</v>
+      </c>
+      <c r="AM75">
+        <v>-7.3</v>
+      </c>
+      <c r="AN75">
+        <v>-9.1</v>
+      </c>
+      <c r="AO75">
+        <v>-3.4</v>
+      </c>
+      <c r="AP75">
+        <v>-7</v>
+      </c>
+      <c r="AQ75">
+        <v>-3.8</v>
+      </c>
+      <c r="AR75">
+        <v>0.3</v>
+      </c>
+      <c r="AS75">
+        <v>2.5</v>
+      </c>
+      <c r="AT75">
+        <v>0.5</v>
+      </c>
+      <c r="AU75">
+        <v>-3.3</v>
+      </c>
+      <c r="AV75">
+        <v>-9.8000000000000007</v>
+      </c>
     </row>
     <row r="76" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A76" s="16">
         <v>45723</v>
       </c>
+      <c r="B76">
+        <v>-19.5</v>
+      </c>
+      <c r="C76">
+        <v>-2.4</v>
+      </c>
+      <c r="D76">
+        <v>-11.6</v>
+      </c>
+      <c r="E76">
+        <v>-6.2</v>
+      </c>
+      <c r="F76">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="G76">
+        <v>-9.3000000000000007</v>
+      </c>
+      <c r="H76">
+        <v>-7.6</v>
+      </c>
+      <c r="I76">
+        <v>-3.4</v>
+      </c>
+      <c r="J76">
+        <v>-4.8</v>
+      </c>
+      <c r="K76" t="s">
+        <v>245</v>
+      </c>
+      <c r="L76">
+        <v>-12.4</v>
+      </c>
+      <c r="M76">
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="N76">
+        <v>-14.7</v>
+      </c>
+      <c r="O76">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="P76">
+        <v>-8.6999999999999993</v>
+      </c>
+      <c r="Q76">
+        <v>-7.9</v>
+      </c>
+      <c r="R76">
+        <v>0.1</v>
+      </c>
+      <c r="S76">
+        <v>-15.5</v>
+      </c>
+      <c r="T76">
+        <v>-10.6</v>
+      </c>
+      <c r="U76">
+        <v>-14.4</v>
+      </c>
+      <c r="V76">
+        <v>-10.4</v>
+      </c>
+      <c r="W76">
+        <v>-3.3</v>
+      </c>
+      <c r="X76">
+        <v>-14.2</v>
+      </c>
+      <c r="Y76">
+        <v>1.2</v>
+      </c>
+      <c r="Z76">
+        <v>-4.2</v>
+      </c>
+      <c r="AA76">
+        <v>-2.5</v>
+      </c>
+      <c r="AB76">
+        <v>-7.1</v>
+      </c>
+      <c r="AC76">
+        <v>6</v>
+      </c>
+      <c r="AD76">
+        <v>8.6</v>
+      </c>
+      <c r="AE76">
+        <v>-15</v>
+      </c>
+      <c r="AF76">
+        <v>4.7</v>
+      </c>
+      <c r="AG76">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AH76">
+        <v>2.4</v>
+      </c>
+      <c r="AI76">
+        <v>3.4</v>
+      </c>
+      <c r="AJ76">
+        <v>6.5</v>
+      </c>
+      <c r="AK76">
+        <v>7.6</v>
+      </c>
+      <c r="AL76">
+        <v>3.5</v>
+      </c>
+      <c r="AM76">
+        <v>-8.6</v>
+      </c>
+      <c r="AN76">
+        <v>-7.7</v>
+      </c>
+      <c r="AO76">
+        <v>-0.7</v>
+      </c>
+      <c r="AP76">
+        <v>-3.7</v>
+      </c>
+      <c r="AQ76">
+        <v>-4.2</v>
+      </c>
+      <c r="AR76">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AS76">
+        <v>5.2</v>
+      </c>
+      <c r="AT76">
+        <v>2</v>
+      </c>
+      <c r="AU76">
+        <v>-1.9</v>
+      </c>
+      <c r="AV76">
+        <v>-8.1999999999999993</v>
+      </c>
     </row>
     <row r="77" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A77" s="16">
         <v>45724</v>
+      </c>
+      <c r="B77">
+        <v>-15.8</v>
+      </c>
+      <c r="C77">
+        <v>1.6</v>
+      </c>
+      <c r="D77">
+        <v>-14.5</v>
+      </c>
+      <c r="E77">
+        <v>-6.5</v>
+      </c>
+      <c r="F77">
+        <v>-14.9</v>
+      </c>
+      <c r="G77">
+        <v>-7.1</v>
+      </c>
+      <c r="H77">
+        <v>-5.6</v>
+      </c>
+      <c r="I77">
+        <v>-5</v>
+      </c>
+      <c r="J77">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="K77" t="s">
+        <v>245</v>
+      </c>
+      <c r="L77">
+        <v>-8.9</v>
+      </c>
+      <c r="M77">
+        <v>-6.6</v>
+      </c>
+      <c r="N77">
+        <v>-11.2</v>
+      </c>
+      <c r="O77">
+        <v>-9</v>
+      </c>
+      <c r="P77">
+        <v>-3.5</v>
+      </c>
+      <c r="Q77">
+        <v>-8</v>
+      </c>
+      <c r="R77">
+        <v>-1.2</v>
+      </c>
+      <c r="S77">
+        <v>-14</v>
+      </c>
+      <c r="T77">
+        <v>-7.7</v>
+      </c>
+      <c r="U77">
+        <v>-14.2</v>
+      </c>
+      <c r="V77">
+        <v>-4.7</v>
+      </c>
+      <c r="W77">
+        <v>-0.5</v>
+      </c>
+      <c r="X77">
+        <v>-9.4</v>
+      </c>
+      <c r="Y77">
+        <v>7.1</v>
+      </c>
+      <c r="Z77">
+        <v>-0.3</v>
+      </c>
+      <c r="AA77">
+        <v>-4.5</v>
+      </c>
+      <c r="AB77">
+        <v>-5.6</v>
+      </c>
+      <c r="AC77">
+        <v>3.5</v>
+      </c>
+      <c r="AD77">
+        <v>5.9</v>
+      </c>
+      <c r="AE77">
+        <v>-6.8</v>
+      </c>
+      <c r="AF77">
+        <v>9</v>
+      </c>
+      <c r="AG77">
+        <v>11.5</v>
+      </c>
+      <c r="AH77">
+        <v>7.3</v>
+      </c>
+      <c r="AI77">
+        <v>2.1</v>
+      </c>
+      <c r="AJ77">
+        <v>6.6</v>
+      </c>
+      <c r="AK77">
+        <v>7.8</v>
+      </c>
+      <c r="AL77">
+        <v>9.4</v>
+      </c>
+      <c r="AM77">
+        <v>-8.5</v>
+      </c>
+      <c r="AN77">
+        <v>-2.4</v>
+      </c>
+      <c r="AO77">
+        <v>-0.6</v>
+      </c>
+      <c r="AP77">
+        <v>-3.8</v>
+      </c>
+      <c r="AQ77">
+        <v>-3.1</v>
+      </c>
+      <c r="AR77">
+        <v>-1.3</v>
+      </c>
+      <c r="AS77">
+        <v>1.6</v>
+      </c>
+      <c r="AT77">
+        <v>2</v>
+      </c>
+      <c r="AU77">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="AV77">
+        <v>-7.7</v>
       </c>
     </row>
     <row r="78" spans="1:48" x14ac:dyDescent="0.4">
@@ -30975,37 +31380,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="67" t="s">
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="68" t="s">
         <v>246</v>
       </c>
-      <c r="E1" s="69">
+      <c r="E1" s="70">
         <v>45715</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="62" t="s">
+      <c r="F1" s="71"/>
+      <c r="G1" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="63"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="73" t="s">
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="74" t="s">
         <v>258</v>
       </c>
-      <c r="H2" s="74"/>
+      <c r="H2" s="75"/>
       <c r="J2" s="23"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:12" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="59"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="51" t="s">
         <v>90</v>
       </c>
@@ -31032,7 +31437,7 @@
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="53"/>
       <c r="C4" s="52" t="s">
         <v>283</v>
@@ -31052,7 +31457,7 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="59"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="53"/>
       <c r="C5" s="52" t="s">
         <v>285</v>
@@ -31070,7 +31475,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="59"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="53"/>
       <c r="C6" s="52" t="s">
         <v>283</v>
@@ -31088,7 +31493,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="59"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="53"/>
       <c r="C7" s="52" t="s">
         <v>283</v>
@@ -31106,7 +31511,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="59"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="53"/>
       <c r="C8" s="52" t="s">
         <v>285</v>
@@ -31124,7 +31529,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="59"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="53"/>
       <c r="C9" s="52" t="s">
         <v>283</v>
@@ -31142,7 +31547,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="59"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="53"/>
       <c r="C10" s="52" t="s">
         <v>283</v>
@@ -31160,7 +31565,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="59"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="53"/>
       <c r="C11" s="52" t="s">
         <v>285</v>
@@ -31178,7 +31583,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="59"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="53"/>
       <c r="C12" s="52" t="s">
         <v>285</v>
@@ -31194,7 +31599,7 @@
       <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="59"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="53"/>
       <c r="C13" s="52" t="s">
         <v>285</v>
@@ -31212,7 +31617,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="59"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="53"/>
       <c r="C14" s="52" t="s">
         <v>285</v>
@@ -31230,7 +31635,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="59"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="53"/>
       <c r="C15" s="52" t="s">
         <v>285</v>
@@ -31248,7 +31653,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="59"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="53"/>
       <c r="C16" s="52" t="s">
         <v>285</v>
@@ -31266,7 +31671,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="59"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="53"/>
       <c r="C17" s="52" t="s">
         <v>285</v>
@@ -31284,7 +31689,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="59"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="53"/>
       <c r="C18" s="52" t="s">
         <v>285</v>
@@ -31302,7 +31707,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="59"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="53"/>
       <c r="C19" s="52" t="s">
         <v>283</v>
@@ -31320,7 +31725,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="59"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="53"/>
       <c r="C20" s="53" t="s">
         <v>284</v>
@@ -31338,7 +31743,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="59"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="53"/>
       <c r="C21" s="52" t="s">
         <v>285</v>
@@ -31356,7 +31761,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="59"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="53"/>
       <c r="C22" s="52" t="s">
         <v>285</v>
@@ -31374,7 +31779,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="59"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="53"/>
       <c r="C23" s="52" t="s">
         <v>285</v>
@@ -31392,7 +31797,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="59"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="53"/>
       <c r="C24" s="52" t="s">
         <v>285</v>
@@ -31408,7 +31813,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="59"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="53"/>
       <c r="C25" s="52" t="s">
         <v>285</v>
@@ -31424,7 +31829,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="59"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="53"/>
       <c r="C26" s="52" t="s">
         <v>285</v>
@@ -31440,7 +31845,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="59"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="53"/>
       <c r="C27" s="52" t="s">
         <v>285</v>
@@ -31456,7 +31861,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="59"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="53"/>
       <c r="C28" s="52" t="s">
         <v>285</v>
@@ -31468,7 +31873,7 @@
       <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="59"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="53"/>
       <c r="C29" s="52" t="s">
         <v>285</v>
@@ -31480,7 +31885,7 @@
       <c r="H29" s="34"/>
     </row>
     <row r="30" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="59"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="53"/>
       <c r="C30" s="52" t="s">
         <v>285</v>
@@ -31492,7 +31897,7 @@
       <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="59"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="53"/>
       <c r="C31" s="52" t="s">
         <v>285</v>
@@ -31504,7 +31909,7 @@
       <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="59"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="53"/>
       <c r="C32" s="52" t="s">
         <v>285</v>
@@ -31516,7 +31921,7 @@
       <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="59"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="53"/>
       <c r="C33" s="52" t="s">
         <v>285</v>
@@ -31528,7 +31933,7 @@
       <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="59"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="53"/>
       <c r="C34" s="52" t="s">
         <v>285</v>
@@ -31540,7 +31945,7 @@
       <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="59"/>
+      <c r="A35" s="60"/>
       <c r="B35" s="53"/>
       <c r="C35" s="52" t="s">
         <v>285</v>
@@ -31552,7 +31957,7 @@
       <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="59"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="53"/>
       <c r="C36" s="52" t="s">
         <v>285</v>
@@ -31564,7 +31969,7 @@
       <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="59"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="53"/>
       <c r="C37" s="52" t="s">
         <v>285</v>
@@ -31576,7 +31981,7 @@
       <c r="H37" s="34"/>
     </row>
     <row r="38" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="59"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="53"/>
       <c r="C38" s="52" t="s">
         <v>285</v>
@@ -31588,7 +31993,7 @@
       <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="59"/>
+      <c r="A39" s="60"/>
       <c r="B39" s="53"/>
       <c r="C39" s="52" t="s">
         <v>285</v>
@@ -31600,7 +32005,7 @@
       <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="59"/>
+      <c r="A40" s="60"/>
       <c r="B40" s="53"/>
       <c r="C40" s="52" t="s">
         <v>285</v>
@@ -31612,7 +32017,7 @@
       <c r="H40" s="34"/>
     </row>
     <row r="41" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="59"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="53"/>
       <c r="C41" s="52" t="s">
         <v>285</v>
@@ -31624,7 +32029,7 @@
       <c r="H41" s="34"/>
     </row>
     <row r="42" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="59"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="53"/>
       <c r="C42" s="52" t="s">
         <v>285</v>
@@ -31636,7 +32041,7 @@
       <c r="H42" s="34"/>
     </row>
     <row r="43" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="59"/>
+      <c r="A43" s="60"/>
       <c r="B43" s="53"/>
       <c r="C43" s="52" t="s">
         <v>285</v>
@@ -31648,7 +32053,7 @@
       <c r="H43" s="34"/>
     </row>
     <row r="44" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="59"/>
+      <c r="A44" s="60"/>
       <c r="B44" s="53"/>
       <c r="C44" s="52" t="s">
         <v>285</v>
@@ -31660,7 +32065,7 @@
       <c r="H44" s="34"/>
     </row>
     <row r="45" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="59"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="53"/>
       <c r="C45" s="52" t="s">
         <v>285</v>
@@ -31672,7 +32077,7 @@
       <c r="H45" s="34"/>
     </row>
     <row r="46" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="59"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="53"/>
       <c r="C46" s="52" t="s">
         <v>285</v>
@@ -31684,7 +32089,7 @@
       <c r="H46" s="34"/>
     </row>
     <row r="47" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="59"/>
+      <c r="A47" s="60"/>
       <c r="B47" s="53"/>
       <c r="C47" s="52" t="s">
         <v>285</v>
@@ -31696,7 +32101,7 @@
       <c r="H47" s="34"/>
     </row>
     <row r="48" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="59"/>
+      <c r="A48" s="60"/>
       <c r="B48" s="53"/>
       <c r="C48" s="52" t="s">
         <v>285</v>
@@ -31708,7 +32113,7 @@
       <c r="H48" s="34"/>
     </row>
     <row r="49" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="59"/>
+      <c r="A49" s="60"/>
       <c r="B49" s="53"/>
       <c r="C49" s="52" t="s">
         <v>285</v>
@@ -31720,7 +32125,7 @@
       <c r="H49" s="34"/>
     </row>
     <row r="50" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="59"/>
+      <c r="A50" s="60"/>
       <c r="B50" s="53"/>
       <c r="C50" s="52" t="s">
         <v>285</v>
@@ -31732,10 +32137,10 @@
       <c r="H50" s="34"/>
     </row>
     <row r="51" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="59"/>
+      <c r="A51" s="60"/>
     </row>
     <row r="52" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="59"/>
+      <c r="A52" s="60"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:H18">
@@ -31784,7 +32189,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -31793,22 +32198,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="75" t="s">
-        <v>288</v>
+      <c r="A1" s="59" t="s">
+        <v>287</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="75" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" s="59" t="s">
         <v>299</v>
-      </c>
-      <c r="D1" s="75" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B2" s="4">
         <v>-27</v>
@@ -31817,13 +32222,13 @@
         <v>-22.6</v>
       </c>
       <c r="D2" s="4">
-        <f>B2-C2</f>
+        <f t="shared" ref="D2:D22" si="0">B2-C2</f>
         <v>-4.3999999999999986</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B3" s="4">
         <v>-26.1</v>
@@ -31832,7 +32237,7 @@
         <v>-27.3</v>
       </c>
       <c r="D3" s="4">
-        <f>B3-C3</f>
+        <f t="shared" si="0"/>
         <v>1.1999999999999993</v>
       </c>
     </row>
@@ -31847,13 +32252,13 @@
         <v>-27.8</v>
       </c>
       <c r="D4" s="4">
-        <f>B4-C4</f>
+        <f t="shared" si="0"/>
         <v>2.4000000000000021</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5" s="4">
         <v>-25.2</v>
@@ -31862,7 +32267,7 @@
         <v>-21.7</v>
       </c>
       <c r="D5" s="4">
-        <f>B5-C5</f>
+        <f t="shared" si="0"/>
         <v>-3.5</v>
       </c>
     </row>
@@ -31877,13 +32282,13 @@
         <v>-27</v>
       </c>
       <c r="D6" s="4">
-        <f>B6-C6</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B7" s="4">
         <v>-24.1</v>
@@ -31892,13 +32297,13 @@
         <v>-24</v>
       </c>
       <c r="D7" s="4">
-        <f>B7-C7</f>
+        <f t="shared" si="0"/>
         <v>-0.10000000000000142</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B8" s="4">
         <v>-24.1</v>
@@ -31907,7 +32312,7 @@
         <v>-23.1</v>
       </c>
       <c r="D8" s="4">
-        <f>B8-C8</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
@@ -31922,13 +32327,13 @@
         <v>-22.9</v>
       </c>
       <c r="D9" s="4">
-        <f>B9-C9</f>
+        <f t="shared" si="0"/>
         <v>-0.80000000000000071</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B10" s="4">
         <v>-23.4</v>
@@ -31937,13 +32342,13 @@
         <v>-26.9</v>
       </c>
       <c r="D10" s="4">
-        <f>B10-C10</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B11" s="4">
         <v>-23.2</v>
@@ -31952,13 +32357,13 @@
         <v>-23.3</v>
       </c>
       <c r="D11" s="4">
-        <f>B11-C11</f>
+        <f t="shared" si="0"/>
         <v>0.10000000000000142</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B12" s="4">
         <v>-22.4</v>
@@ -31967,7 +32372,7 @@
         <v>-26.6</v>
       </c>
       <c r="D12" s="4">
-        <f>B12-C12</f>
+        <f t="shared" si="0"/>
         <v>4.2000000000000028</v>
       </c>
     </row>
@@ -31982,7 +32387,7 @@
         <v>-23.3</v>
       </c>
       <c r="D13" s="4">
-        <f>B13-C13</f>
+        <f t="shared" si="0"/>
         <v>1.3000000000000007</v>
       </c>
     </row>
@@ -31997,7 +32402,7 @@
         <v>-20.6</v>
       </c>
       <c r="D14" s="4">
-        <f>B14-C14</f>
+        <f t="shared" si="0"/>
         <v>-1.1999999999999993</v>
       </c>
     </row>
@@ -32012,7 +32417,7 @@
         <v>-25.1</v>
       </c>
       <c r="D15" s="4">
-        <f>B15-C15</f>
+        <f t="shared" si="0"/>
         <v>3.4000000000000021</v>
       </c>
     </row>
@@ -32027,13 +32432,13 @@
         <v>-23.5</v>
       </c>
       <c r="D16" s="4">
-        <f>B16-C16</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B17" s="4">
         <v>-20</v>
@@ -32042,7 +32447,7 @@
         <v>-23.6</v>
       </c>
       <c r="D17" s="4">
-        <f>B17-C17</f>
+        <f t="shared" si="0"/>
         <v>3.6000000000000014</v>
       </c>
     </row>
@@ -32057,7 +32462,7 @@
         <v>-23.4</v>
       </c>
       <c r="D18" s="4">
-        <f>B18-C18</f>
+        <f t="shared" si="0"/>
         <v>3.7999999999999972</v>
       </c>
     </row>
@@ -32072,13 +32477,13 @@
         <v>-22</v>
       </c>
       <c r="D19" s="4">
-        <f>B19-C19</f>
+        <f t="shared" si="0"/>
         <v>3.1000000000000014</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B20" s="4">
         <v>-18.8</v>
@@ -32087,7 +32492,7 @@
         <v>-23.1</v>
       </c>
       <c r="D20" s="4">
-        <f>B20-C20</f>
+        <f t="shared" si="0"/>
         <v>4.3000000000000007</v>
       </c>
     </row>
@@ -32102,13 +32507,13 @@
         <v>-19.399999999999999</v>
       </c>
       <c r="D21" s="4">
-        <f>B21-C21</f>
+        <f t="shared" si="0"/>
         <v>1.1999999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B22" s="4">
         <v>-16.2</v>
@@ -32117,7 +32522,7 @@
         <v>-16.2</v>
       </c>
       <c r="D22" s="4">
-        <f>B22-C22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -32126,17 +32531,17 @@
     <sortCondition ref="B2:B22"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D22">
-    <cfRule type="top10" dxfId="10" priority="6" rank="1"/>
-    <cfRule type="top10" dxfId="9" priority="5" bottom="1" rank="1"/>
+  <conditionalFormatting sqref="B2:B22">
+    <cfRule type="top10" dxfId="5" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C22">
-    <cfRule type="top10" dxfId="8" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="7" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B22">
-    <cfRule type="top10" dxfId="2" priority="2" rank="1"/>
-    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
+  <conditionalFormatting sqref="D2:D22">
+    <cfRule type="top10" dxfId="1" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="6" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>